<commit_message>
- add column {NapCoc, SuDungCoc, SoDuCoc}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhSachNhaCungCap.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhSachNhaCungCap.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Điện thoại</t>
   </si>
@@ -52,13 +52,19 @@
     <t>Người tạo</t>
   </si>
   <si>
-    <t>Chi phí DV ngoài</t>
-  </si>
-  <si>
     <t>Tỉnh thành</t>
   </si>
   <si>
     <t>Quận huyện</t>
+  </si>
+  <si>
+    <t>Tổng nạp cọc</t>
+  </si>
+  <si>
+    <t>Sử dụng cọc</t>
+  </si>
+  <si>
+    <t>Số dư cọc</t>
   </si>
 </sst>
 </file>
@@ -562,11 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,13 +585,13 @@
     <col min="6" max="6" width="37.140625" style="14" customWidth="1"/>
     <col min="7" max="7" width="29" style="11" customWidth="1"/>
     <col min="8" max="9" width="17.42578125" style="11" customWidth="1"/>
-    <col min="10" max="11" width="21.5703125" style="19" customWidth="1"/>
-    <col min="12" max="12" width="18" style="19" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="13" width="21.5703125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="18" style="19" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
@@ -601,9 +607,11 @@
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="3" spans="1:16" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -623,10 +631,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>10</v>
@@ -638,13 +646,19 @@
         <v>7</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9"/>
       <c r="C4" s="6"/>
@@ -657,9 +671,11 @@
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="9"/>
       <c r="C5" s="6"/>
@@ -672,9 +688,11 @@
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6"/>
@@ -687,9 +705,11 @@
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="9"/>
       <c r="C7" s="6"/>
@@ -702,9 +722,11 @@
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="9"/>
       <c r="C8" s="6"/>
@@ -717,9 +739,11 @@
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="9"/>
       <c r="C9" s="6"/>
@@ -732,9 +756,11 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
       <c r="C10" s="6"/>
@@ -747,9 +773,11 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="9"/>
       <c r="C11" s="6"/>
@@ -762,9 +790,11 @@
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6"/>
@@ -777,9 +807,11 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6"/>
@@ -792,9 +824,11 @@
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
@@ -807,9 +841,11 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
@@ -822,9 +858,11 @@
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
@@ -837,9 +875,11 @@
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
@@ -852,9 +892,11 @@
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
@@ -867,9 +909,11 @@
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
@@ -882,9 +926,11 @@
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
@@ -897,9 +943,11 @@
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
@@ -912,9 +960,11 @@
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
@@ -927,9 +977,11 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
@@ -942,9 +994,11 @@
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
@@ -957,9 +1011,11 @@
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
@@ -972,9 +1028,11 @@
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
@@ -987,9 +1045,11 @@
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
@@ -1002,9 +1062,11 @@
       <c r="J27" s="22"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="23"/>
       <c r="C28" s="26"/>
@@ -1026,11 +1088,19 @@
         <f>SUM(L$4:L27)</f>
         <v>0</v>
       </c>
-      <c r="M28" s="15"/>
+      <c r="M28" s="18">
+        <f>SUM(M$4:M27)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="18">
+        <f>SUM(N$4:N27)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>